<commit_message>
Modificación del archivo data/state.json
</commit_message>
<xml_diff>
--- a/data/output/Pedido_Semana_14_2026-02-03_deco_interior.xlsx
+++ b/data/output/Pedido_Semana_14_2026-02-03_deco_interior.xlsx
@@ -1316,10 +1316,10 @@
         <v>1</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M13" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="4" t="n">
         <v>7.5</v>
@@ -1382,10 +1382,10 @@
         <v>2</v>
       </c>
       <c r="L14" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M14" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="4" t="n">
         <v>67.8</v>
@@ -1514,10 +1514,10 @@
         <v>1</v>
       </c>
       <c r="L16" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M16" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="4" t="n">
         <v>19.5</v>
@@ -1778,10 +1778,10 @@
         <v>2</v>
       </c>
       <c r="L20" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M20" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N20" s="4" t="n">
         <v>10</v>
@@ -1844,10 +1844,10 @@
         <v>3</v>
       </c>
       <c r="L21" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M21" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="4" t="n">
         <v>15.75</v>
@@ -2042,10 +2042,10 @@
         <v>3</v>
       </c>
       <c r="L24" s="3" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M24" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N24" s="4" t="n">
         <v>10.35</v>
@@ -2108,10 +2108,10 @@
         <v>2</v>
       </c>
       <c r="L25" s="3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M25" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N25" s="4" t="n">
         <v>9.949999999999999</v>
@@ -2174,10 +2174,10 @@
         <v>3</v>
       </c>
       <c r="L26" s="3" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M26" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N26" s="4" t="n">
         <v>5.4</v>
@@ -2240,10 +2240,10 @@
         <v>2</v>
       </c>
       <c r="L27" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M27" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N27" s="4" t="n">
         <v>5</v>
@@ -2438,10 +2438,10 @@
         <v>4</v>
       </c>
       <c r="L30" s="3" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M30" s="3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N30" s="4" t="n">
         <v>11.05</v>
@@ -2504,10 +2504,10 @@
         <v>2</v>
       </c>
       <c r="L31" s="3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M31" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N31" s="4" t="n">
         <v>3.9</v>
@@ -3560,10 +3560,10 @@
         <v>1</v>
       </c>
       <c r="L47" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M47" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N47" s="4" t="n">
         <v>5.99</v>
@@ -4154,10 +4154,10 @@
         <v>3</v>
       </c>
       <c r="L56" s="3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M56" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N56" s="4" t="n">
         <v>13.65</v>
@@ -4748,10 +4748,10 @@
         <v>1</v>
       </c>
       <c r="L65" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M65" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N65" s="4" t="n">
         <v>11.97</v>
@@ -5210,10 +5210,10 @@
         <v>1</v>
       </c>
       <c r="L72" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M72" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N72" s="4" t="n">
         <v>1.45</v>
@@ -5342,10 +5342,10 @@
         <v>1</v>
       </c>
       <c r="L74" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M74" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N74" s="4" t="n">
         <v>3.95</v>
@@ -5672,10 +5672,10 @@
         <v>2</v>
       </c>
       <c r="L79" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M79" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N79" s="4" t="n">
         <v>37.8</v>
@@ -6200,10 +6200,10 @@
         <v>2</v>
       </c>
       <c r="L87" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M87" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N87" s="4" t="n">
         <v>56.94</v>
@@ -6794,10 +6794,10 @@
         <v>3</v>
       </c>
       <c r="L96" s="3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M96" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N96" s="4" t="n">
         <v>13.93</v>
@@ -7058,10 +7058,10 @@
         <v>1</v>
       </c>
       <c r="L100" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M100" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N100" s="4" t="n">
         <v>7.99</v>
@@ -7388,10 +7388,10 @@
         <v>1</v>
       </c>
       <c r="L105" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M105" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N105" s="4" t="n">
         <v>4.99</v>
@@ -7652,10 +7652,10 @@
         <v>2</v>
       </c>
       <c r="L109" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M109" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N109" s="4" t="n">
         <v>35.96</v>
@@ -7718,10 +7718,10 @@
         <v>3</v>
       </c>
       <c r="L110" s="3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M110" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N110" s="4" t="n">
         <v>76.93000000000001</v>
@@ -7982,10 +7982,10 @@
         <v>1</v>
       </c>
       <c r="L114" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M114" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N114" s="4" t="n">
         <v>5.99</v>
@@ -8576,10 +8576,10 @@
         <v>1</v>
       </c>
       <c r="L123" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M123" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N123" s="4" t="n">
         <v>3.9</v>
@@ -8906,10 +8906,10 @@
         <v>1</v>
       </c>
       <c r="L128" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M128" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N128" s="4" t="n">
         <v>13</v>
@@ -9104,10 +9104,10 @@
         <v>1</v>
       </c>
       <c r="L131" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M131" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N131" s="4" t="n">
         <v>6.5</v>
@@ -9465,7 +9465,7 @@
         </is>
       </c>
       <c r="C139" s="8" t="n">
-        <v>334</v>
+        <v>372</v>
       </c>
     </row>
     <row r="140">
@@ -9585,7 +9585,7 @@
         </is>
       </c>
       <c r="C150" s="8" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hemos hecho modificaciones en el resumen_pedido para que aparezcan todas las secciones
</commit_message>
<xml_diff>
--- a/data/output/Pedido_Semana_14_2026-02-03_deco_interior.xlsx
+++ b/data/output/Pedido_Semana_14_2026-02-03_deco_interior.xlsx
@@ -1316,10 +1316,10 @@
         <v>1</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M13" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="4" t="n">
         <v>7.5</v>
@@ -1382,10 +1382,10 @@
         <v>2</v>
       </c>
       <c r="L14" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M14" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="4" t="n">
         <v>67.8</v>
@@ -1514,10 +1514,10 @@
         <v>1</v>
       </c>
       <c r="L16" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M16" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="4" t="n">
         <v>19.5</v>
@@ -1778,10 +1778,10 @@
         <v>2</v>
       </c>
       <c r="L20" s="3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M20" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N20" s="4" t="n">
         <v>10</v>
@@ -1844,10 +1844,10 @@
         <v>3</v>
       </c>
       <c r="L21" s="3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M21" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21" s="4" t="n">
         <v>15.75</v>
@@ -2042,10 +2042,10 @@
         <v>3</v>
       </c>
       <c r="L24" s="3" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="M24" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N24" s="4" t="n">
         <v>10.35</v>
@@ -2108,10 +2108,10 @@
         <v>2</v>
       </c>
       <c r="L25" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M25" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N25" s="4" t="n">
         <v>9.949999999999999</v>
@@ -2174,10 +2174,10 @@
         <v>3</v>
       </c>
       <c r="L26" s="3" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="M26" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N26" s="4" t="n">
         <v>5.4</v>
@@ -2240,10 +2240,10 @@
         <v>2</v>
       </c>
       <c r="L27" s="3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M27" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N27" s="4" t="n">
         <v>5</v>
@@ -2438,10 +2438,10 @@
         <v>4</v>
       </c>
       <c r="L30" s="3" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M30" s="3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N30" s="4" t="n">
         <v>11.05</v>
@@ -2504,10 +2504,10 @@
         <v>2</v>
       </c>
       <c r="L31" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M31" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N31" s="4" t="n">
         <v>3.9</v>
@@ -3560,10 +3560,10 @@
         <v>1</v>
       </c>
       <c r="L47" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M47" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N47" s="4" t="n">
         <v>5.99</v>
@@ -4154,10 +4154,10 @@
         <v>3</v>
       </c>
       <c r="L56" s="3" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M56" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N56" s="4" t="n">
         <v>13.65</v>
@@ -4748,10 +4748,10 @@
         <v>1</v>
       </c>
       <c r="L65" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M65" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N65" s="4" t="n">
         <v>11.97</v>
@@ -5210,10 +5210,10 @@
         <v>1</v>
       </c>
       <c r="L72" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M72" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N72" s="4" t="n">
         <v>1.45</v>
@@ -5342,10 +5342,10 @@
         <v>1</v>
       </c>
       <c r="L74" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M74" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N74" s="4" t="n">
         <v>3.95</v>
@@ -5672,10 +5672,10 @@
         <v>2</v>
       </c>
       <c r="L79" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M79" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N79" s="4" t="n">
         <v>37.8</v>
@@ -6200,10 +6200,10 @@
         <v>2</v>
       </c>
       <c r="L87" s="3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M87" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N87" s="4" t="n">
         <v>56.94</v>
@@ -6794,10 +6794,10 @@
         <v>3</v>
       </c>
       <c r="L96" s="3" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M96" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N96" s="4" t="n">
         <v>13.93</v>
@@ -7058,10 +7058,10 @@
         <v>1</v>
       </c>
       <c r="L100" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M100" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N100" s="4" t="n">
         <v>7.99</v>
@@ -7388,10 +7388,10 @@
         <v>1</v>
       </c>
       <c r="L105" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M105" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N105" s="4" t="n">
         <v>4.99</v>
@@ -7652,10 +7652,10 @@
         <v>2</v>
       </c>
       <c r="L109" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M109" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N109" s="4" t="n">
         <v>35.96</v>
@@ -7718,10 +7718,10 @@
         <v>3</v>
       </c>
       <c r="L110" s="3" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M110" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N110" s="4" t="n">
         <v>76.93000000000001</v>
@@ -7982,10 +7982,10 @@
         <v>1</v>
       </c>
       <c r="L114" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M114" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N114" s="4" t="n">
         <v>5.99</v>
@@ -8576,10 +8576,10 @@
         <v>1</v>
       </c>
       <c r="L123" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M123" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N123" s="4" t="n">
         <v>3.9</v>
@@ -8906,10 +8906,10 @@
         <v>1</v>
       </c>
       <c r="L128" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M128" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N128" s="4" t="n">
         <v>13</v>
@@ -9104,10 +9104,10 @@
         <v>1</v>
       </c>
       <c r="L131" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M131" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N131" s="4" t="n">
         <v>6.5</v>
@@ -9465,7 +9465,7 @@
         </is>
       </c>
       <c r="C139" s="8" t="n">
-        <v>372</v>
+        <v>334</v>
       </c>
     </row>
     <row r="140">
@@ -9585,7 +9585,7 @@
         </is>
       </c>
       <c r="C150" s="8" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>